<commit_message>
Cambio Solicitud Gráfica MA_07_13_CO_REC50
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion13/MA_07_13_CO_REC50.xlsx
+++ b/fuentes/contenidos/grado07/guion13/MA_07_13_CO_REC50.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Copia\JOHANNA\Documents\Documents\Matematicas\fuentes\contenidos\grado07\guion13\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8955" tabRatio="500"/>
@@ -16,7 +21,7 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
 </workbook>
 </file>
 
@@ -618,9 +623,6 @@
     <t>MA_07_13_CO_RE50</t>
   </si>
   <si>
-    <t xml:space="preserve">Esta fila no se me dejó editar en la parte de la descripción, por lo tanto se pasa a la siguiente. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Imagen con dos poliedros, uno cóncavo y el otro convexo en medio de los dos poliedros un signo de pregunta. </t>
   </si>
   <si>
@@ -631,6 +633,9 @@
   </si>
   <si>
     <t xml:space="preserve">Se adjunta imagen guía, aunque los poliedros pueden ser cualquieras siempre y cuando el 2 y 3 sean cóncavos. </t>
+  </si>
+  <si>
+    <t> 231673213</t>
   </si>
 </sst>
 </file>
@@ -1296,7 +1301,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1348,8 +1353,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1670,8 +1676,9 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="52">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1697,6 +1704,7 @@
     <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="51" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -2134,7 +2142,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2142,6 +2150,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2175,7 +2197,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2183,6 +2205,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2216,7 +2252,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2224,6 +2260,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2257,7 +2307,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2265,6 +2315,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2298,7 +2362,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2306,6 +2370,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2339,7 +2417,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2347,6 +2425,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2380,7 +2472,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2388,6 +2480,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2723,9 +2829,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3175,10 +3281,10 @@
         <v>500 x 500 px</v>
       </c>
       <c r="J13" s="64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K13" s="64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
@@ -3221,20 +3327,20 @@
         <v>196</v>
       </c>
       <c r="K14" s="64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
       </c>
-      <c r="B15" s="62" t="s">
-        <v>198</v>
+      <c r="B15" s="109" t="s">
+        <v>202</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3302,10 +3408,10 @@
         <v>500 x 500 px</v>
       </c>
       <c r="J16" s="67" t="s">
+        <v>199</v>
+      </c>
+      <c r="K16" s="68" t="s">
         <v>200</v>
-      </c>
-      <c r="K16" s="68" t="s">
-        <v>201</v>
       </c>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
@@ -6240,9 +6346,12 @@
       <formula1>$O$2:$O$27</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1" display="http://www.shutterstock.com/pic-231673213/stock-photo-octahedron-shaped-die-england-uk-western-europe.html?src=8_meLTtYN2LbV6Wxn62ZFw-1-16"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>